<commit_message>
Fix for bug in how Previously Visited positions were marked.
</commit_message>
<xml_diff>
--- a/GeoCacheProblem/GridWithValues.xlsx
+++ b/GeoCacheProblem/GridWithValues.xlsx
@@ -1,21 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Develop\Challenges\GeoCacheProblem\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25515" windowHeight="9510"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="9516" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -329,7 +325,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -339,11 +335,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1">
@@ -850,7 +846,7 @@
       <selection activeCell="B1" sqref="A1:B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
@@ -951,4 +947,64 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>9</v>
+      </c>
+      <c r="F2">
+        <v>6</v>
+      </c>
+      <c r="G2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>